<commit_message>
added info for equal metric results
</commit_message>
<xml_diff>
--- a/prioritization/tests/test_input.xlsx
+++ b/prioritization/tests/test_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrahovac/repos/cfh_task_4/prioritization/prioritization/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrahovac/repos/public/QUOP/prioritization/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F22F80-A49F-4B4D-802E-CC168F70C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279E8056-3687-E149-AEB7-638190231F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40320" windowHeight="25100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48580" yWindow="-6080" windowWidth="46520" windowHeight="29600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -72,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Sample Size</t>
   </si>
@@ -288,6 +291,9 @@
   </si>
   <si>
     <t>The code will know which layer_1 or layer_0 it is looking at based on the 1st column header. As there are more than one layer_0 and layer_1 tables, those further tables can have any additions to the table name string, for example layer_1_second_set_of_priority_weights</t>
+  </si>
+  <si>
+    <t>To avoid division zero: If all Layer 0 results are mutually equal, then the Low and the High filters should be such that all options get the same score, so for example, if all results are 0, then one could use -1 and 1 to have all scores be exactly between the Low and the High Score, as given in the table below. Similarly if one prefers to have the score of 1, then the low limit should be set to 0 and the high to, say, 10.</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1255,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:J18"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1273,6 +1279,9 @@
     <row r="4" spans="3:10" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
       </c>
       <c r="G4" t="s">
         <v>51</v>

</xml_diff>